<commit_message>
commit for first push
</commit_message>
<xml_diff>
--- a/data/Satellite_HS_Salmon_18C_Table.xlsx
+++ b/data/Satellite_HS_Salmon_18C_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Dempsey\Desktop\RProjects\coastal_classification\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C185DF70-F947-4C05-A898-3223BF07E0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADFCCCC-4F16-4479-AA92-CE7AC5BFC67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1530" windowWidth="21600" windowHeight="11385" xr2:uid="{2AF08721-EECC-47B2-830D-C110EB8CF113}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AF08721-EECC-47B2-830D-C110EB8CF113}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,25 +104,25 @@
     <t>Cumberland</t>
   </si>
   <si>
-    <t>sat1</t>
-  </si>
-  <si>
-    <t>sat2</t>
-  </si>
-  <si>
-    <t>sat3</t>
-  </si>
-  <si>
-    <t>sat4</t>
-  </si>
-  <si>
-    <t>sat5</t>
-  </si>
-  <si>
-    <t>sat6</t>
-  </si>
-  <si>
-    <t>sat7</t>
+    <t>sat_1</t>
+  </si>
+  <si>
+    <t>sat_2</t>
+  </si>
+  <si>
+    <t>sat_3</t>
+  </si>
+  <si>
+    <t>sat_4</t>
+  </si>
+  <si>
+    <t>sat_5</t>
+  </si>
+  <si>
+    <t>sat_6</t>
+  </si>
+  <si>
+    <t>sat_7</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>